<commit_message>
Build v1.7.2: Cumulative Refactor - Preferences UI, Roundtrip Logic, AppData Rename, Fix Process Kill, SWIFT Metadata
</commit_message>
<xml_diff>
--- a/Imported Templates/$index.xlsx
+++ b/Imported Templates/$index.xlsx
@@ -248,7 +248,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -330,9 +330,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -842,7 +839,7 @@
           <t>filename pattern</t>
         </is>
       </c>
-      <c r="B10" s="30" t="inlineStr"/>
+      <c r="B10" s="26" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>